<commit_message>
Minor chaange in test data for website feedback so as to test Jekins polling
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/websiteFeedback.xlsx
+++ b/src/test/resources/testData/websiteFeedback.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testing\WebTesting\WebTesting\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bajwauto\Projects\Webtesting\WebTesting\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6644C2-0467-411C-8F94-55CD15D0637E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E2BD8A-BCCE-40F0-9B8D-1ECFC45E1CC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Rating</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Dissatisfied</t>
+  </si>
+  <si>
+    <t>Don't ask If I am a bot or not</t>
   </si>
 </sst>
 </file>
@@ -386,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,9 +444,20 @@
       </c>
       <c r="D3" s="2"/>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3" xr:uid="{68A851FB-FE31-4039-B2D3-864CA68DD251}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4" xr:uid="{68A851FB-FE31-4039-B2D3-864CA68DD251}">
       <formula1>"Very Dissatisfied,Dissatisfied,Neutral,Satisfied,Very Satisfied"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Minor data change for the websitefeedback test
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/websiteFeedback.xlsx
+++ b/src/test/resources/testData/websiteFeedback.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Bajwauto\Projects\Webtesting\WebTesting\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E2BD8A-BCCE-40F0-9B8D-1ECFC45E1CC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF793D6-1D72-40A3-B45F-BF6647092B45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,6 +454,7 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="D4" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>